<commit_message>
complete parallel local and fix bug
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieutt\Desktop\PlaywrightLibary\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261C8E26-E91E-4ED3-9D09-E9956C4AACAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CD06DE-EA6B-4B7C-B0DD-2AE90876A4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sitedeclaration" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Env</t>
   </si>
@@ -66,23 +66,68 @@
     <t>MyProject</t>
   </si>
   <si>
-    <t>/fab</t>
-  </si>
-  <si>
     <t>/work</t>
   </si>
   <si>
-    <t>/services</t>
-  </si>
-  <si>
     <t>https://www.gravityglobal.com</t>
+  </si>
+  <si>
+    <t>/about</t>
+  </si>
+  <si>
+    <t>/careers</t>
+  </si>
+  <si>
+    <t>/news</t>
+  </si>
+  <si>
+    <t>/contact</t>
+  </si>
+  <si>
+    <t>/services/account-based-marketing-abm</t>
+  </si>
+  <si>
+    <t>/services/research</t>
+  </si>
+  <si>
+    <t>/services/public-relations</t>
+  </si>
+  <si>
+    <t>/services/creative-content</t>
+  </si>
+  <si>
+    <t>/services/digital/user-experience-optimization</t>
+  </si>
+  <si>
+    <t>/services/digital/digital-design</t>
+  </si>
+  <si>
+    <t>/services/digital/website-development</t>
+  </si>
+  <si>
+    <t>/services/digital/crm</t>
+  </si>
+  <si>
+    <t>/services/account-based-marketing-abm/abm-strategy-and-programs</t>
+  </si>
+  <si>
+    <t>/services/go-to-market/performance-marketing</t>
+  </si>
+  <si>
+    <t>/about/leadership</t>
+  </si>
+  <si>
+    <t>/locations</t>
+  </si>
+  <si>
+    <t>/services/media/paid-search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +161,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,12 +207,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -179,8 +233,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCC7D407-2C14-4F88-AF2B-DAD10F844417}" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{DCC7D407-2C14-4F88-AF2B-DAD10F844417}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCC7D407-2C14-4F88-AF2B-DAD10F844417}" name="Table2" displayName="Table2" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{DCC7D407-2C14-4F88-AF2B-DAD10F844417}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C225A89D-F9F8-4876-975C-8860000132DD}" name="Env"/>
     <tableColumn id="2" xr3:uid="{C1C0E1EA-36E1-4248-AF5B-9B2B79686D8D}" name="Project Name"/>
@@ -519,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F74D42-87B5-479A-8715-DA3CCE7BCBA7}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,11 +610,14 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -578,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,24 +655,103 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
@@ -629,12 +765,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF442BD62CE3614F82B8712B06631535" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="adaefcf9af4e61dfbacd59f14deff25e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="47f9b71a-da86-4a06-a0d0-efb8d1f984f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="610a31c8f17190a4e43c9d63e45c82c7" ns2:_="">
     <xsd:import namespace="47f9b71a-da86-4a06-a0d0-efb8d1f984f9"/>
@@ -778,6 +908,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -788,15 +924,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2A9092A-36BA-4066-93BB-597D83379E3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93B9991E-296C-4E88-B4A7-2749FBC93293}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -814,6 +941,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2A9092A-36BA-4066-93BB-597D83379E3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8318C716-250E-42EA-8E09-58536703EC53}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix data all placeholder
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieutt\Desktop\PlaywrightLibary\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C37A282-BFB1-4038-924A-C134ABA8B65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93B67AE-16BA-4257-A6B6-9957A74AED85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Env</t>
   </si>
@@ -66,61 +66,13 @@
     <t>MyProject</t>
   </si>
   <si>
+    <t>https://www.gravityglobal.com</t>
+  </si>
+  <si>
+    <t>/services</t>
+  </si>
+  <si>
     <t>/work</t>
-  </si>
-  <si>
-    <t>https://www.gravityglobal.com</t>
-  </si>
-  <si>
-    <t>/about</t>
-  </si>
-  <si>
-    <t>/careers</t>
-  </si>
-  <si>
-    <t>/news</t>
-  </si>
-  <si>
-    <t>/contact</t>
-  </si>
-  <si>
-    <t>/services/account-based-marketing-abm</t>
-  </si>
-  <si>
-    <t>/services/research</t>
-  </si>
-  <si>
-    <t>/services/public-relations</t>
-  </si>
-  <si>
-    <t>/services/creative-content</t>
-  </si>
-  <si>
-    <t>/services/digital/user-experience-optimization</t>
-  </si>
-  <si>
-    <t>/services/digital/digital-design</t>
-  </si>
-  <si>
-    <t>/services/digital/website-development</t>
-  </si>
-  <si>
-    <t>/services/digital/crm</t>
-  </si>
-  <si>
-    <t>/services/account-based-marketing-abm/abm-strategy-and-programs</t>
-  </si>
-  <si>
-    <t>/services/go-to-market/performance-marketing</t>
-  </si>
-  <si>
-    <t>/about/leadership</t>
-  </si>
-  <si>
-    <t>/locations</t>
-  </si>
-  <si>
-    <t>/services/media/paid-search</t>
   </si>
 </sst>
 </file>
@@ -576,7 +528,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -635,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,103 +607,19 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
+      <c r="B17" s="4"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>

</xml_diff>